<commit_message>
fix pattern distribution according to new feedback
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboards.xlsx
+++ b/meta/Foundation Model Leaderboards.xlsx
@@ -13,6 +13,7 @@
     <sheet state="visible" name="Missing Entity" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Redundant Entity" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="Unresponsive Entity" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Uncategorized" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -25,6 +26,12 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D199">
+      <text>
+        <t xml:space="preserve">https://github.com/open-compass/MathBench/issues/7
+	-Jimmy Chou</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="H199">
       <text>
         <t xml:space="preserve">https://arxiv.org/pdf/2405.12209
@@ -2340,7 +2347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="934">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -5151,6 +5158,9 @@
   </si>
   <si>
     <t>https://huggingface.co/spaces/OpenGVLab/MVBench_Leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://github.com/open-compass/MathBench/issues/5</t>
   </si>
 </sst>
 </file>
@@ -5318,6 +5328,10 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -9114,8 +9128,8 @@
       <c r="C199" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D199" s="2" t="s">
-        <v>116</v>
+      <c r="D199" s="2">
+        <v>2.0</v>
       </c>
       <c r="E199" s="2" t="s">
         <v>12</v>
@@ -15645,6 +15659,29 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>933</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
add new smell examples
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboards.xlsx
+++ b/meta/Foundation Model Leaderboards.xlsx
@@ -2362,7 +2362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="949">
   <si>
     <t>Leaderboard name</t>
   </si>
@@ -4719,6 +4719,9 @@
     <t>https://github.com/open-compass/opencompass/discussions/784</t>
   </si>
   <si>
+    <t>https://github.com/stanford-crfm/fmti/issues/2</t>
+  </si>
+  <si>
     <t>https://github.com/open-compass/LawBench/issues/7</t>
   </si>
   <si>
@@ -4737,91 +4740,91 @@
     <t>https://github.com/open-compass/opencompass/discussions/785</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/hallucinations-leaderboard/leaderboard/discussions/20</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/livecodebench/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Agent/issues/8</t>
+  </si>
+  <si>
+    <t>https://github.com/TheoremOne/llm-benchmarker-suite/issues/9</t>
+  </si>
+  <si>
+    <t>https://github.com/jeinlee1991/chinese-llm-benchmark/issues/19</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenGVLab/LAMM/issues/64</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/SeaEval/SeaEval_Leaderboard/discussions/2</t>
   </si>
   <si>
-    <t>https://huggingface.co/spaces/hallucinations-leaderboard/leaderboard/discussions/20</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/livecodebench/leaderboard/discussions/1</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Agent/issues/8</t>
-  </si>
-  <si>
-    <t>https://github.com/TheoremOne/llm-benchmarker-suite/issues/9</t>
-  </si>
-  <si>
-    <t>https://github.com/jeinlee1991/chinese-llm-benchmark/issues/19</t>
-  </si>
-  <si>
-    <t>https://github.com/OpenGVLab/LAMM/issues/64</t>
+    <t>https://huggingface.co/spaces/LanguageBind/Video-Bench/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/mike-ravkine/can-ai-code-results/discussions/4</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Auto/issues/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/28</t>
+  </si>
+  <si>
+    <t>https://github.com/microsoft/promptbench/issues/26</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2028</t>
   </si>
   <si>
     <t>https://paperswithcode.com/sota/chat-based-image-retrieval-on-visdial</t>
   </si>
   <si>
-    <t>https://huggingface.co/spaces/LanguageBind/Video-Bench/discussions/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/mike-ravkine/can-ai-code-results/discussions/4</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Auto/issues/3</t>
-  </si>
-  <si>
-    <t>https://huggingface.co/spaces/upstage/open-ko-llm-leaderboard/discussions/28</t>
-  </si>
-  <si>
-    <t>https://github.com/microsoft/promptbench/issues/26</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2028</t>
+    <t>https://huggingface.co/spaces/mike-ravkine/can-ai-code-results/discussions/6</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Code3/issues/3</t>
+  </si>
+  <si>
+    <t>https://github.com/nyu-mll/jiant/issues/1366</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2062</t>
   </si>
   <si>
     <t>https://paperswithcode.com/sota/chinese-reading-comprehension-on-cmrc-2019</t>
   </si>
   <si>
-    <t>https://huggingface.co/spaces/mike-ravkine/can-ai-code-results/discussions/6</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Code3/issues/3</t>
-  </si>
-  <si>
-    <t>https://github.com/nyu-mll/jiant/issues/1366</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2062</t>
+    <t>https://leaderboard.allenai.org/scifact/submission/ce0cbc2odv44t2mapeu0</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Industry/issues/1</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2350</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2358</t>
   </si>
   <si>
     <t>https://paperswithcode.com/sota/zero-shot-dense-video-captioning-on-vitt</t>
   </si>
   <si>
-    <t>https://leaderboard.allenai.org/scifact/submission/ce0cbc2odv44t2mapeu0</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Industry/issues/1</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2350</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2358</t>
+    <t>https://paperswithcode.com/sota/speaker-verification-on-callhome</t>
+  </si>
+  <si>
+    <t>https://github.com/CLUEbenchmark/SuperCLUE-Math6/issues/1</t>
+  </si>
+  <si>
+    <t>https://github.com/TheoremOne/llm-benchmarker-suite/issues/10</t>
+  </si>
+  <si>
+    <t>https://github.com/stanford-crfm/helm/issues/2441</t>
   </si>
   <si>
     <t>https://paperswithcode.com/sota/zero-shot-dense-video-captioning-on-youcook2</t>
-  </si>
-  <si>
-    <t>https://paperswithcode.com/sota/speaker-verification-on-callhome</t>
-  </si>
-  <si>
-    <t>https://github.com/CLUEbenchmark/SuperCLUE-Math6/issues/1</t>
-  </si>
-  <si>
-    <t>https://github.com/TheoremOne/llm-benchmarker-suite/issues/10</t>
-  </si>
-  <si>
-    <t>https://github.com/stanford-crfm/helm/issues/2441</t>
   </si>
   <si>
     <t>https://github.com/CLUEbenchmark/SuperCLUE-RAG/issues/2</t>
@@ -15752,15 +15755,15 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -15788,27 +15791,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="20" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
   </sheetData>
@@ -15967,30 +15970,30 @@
         <v>780</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>766</v>
+        <v>781</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>786</v>
-      </c>
-      <c r="D3" s="16" t="s">
         <v>787</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>766</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>788</v>
@@ -16012,7 +16015,7 @@
       <c r="C4" s="16" t="s">
         <v>793</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="16" t="s">
         <v>794</v>
       </c>
       <c r="E4" s="16" t="s">
@@ -16035,7 +16038,7 @@
       <c r="C5" s="16" t="s">
         <v>800</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="8" t="s">
         <v>801</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -16055,7 +16058,7 @@
       <c r="C6" s="8" t="s">
         <v>805</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="16" t="s">
         <v>806</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -16089,19 +16092,22 @@
       <c r="C8" s="16" t="s">
         <v>815</v>
       </c>
+      <c r="D8" s="8" t="s">
+        <v>816</v>
+      </c>
       <c r="G8" s="8" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="8" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="10">
@@ -16109,10 +16115,10 @@
         <v>770</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="11">
@@ -16120,94 +16126,94 @@
         <v>767</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="8" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="16" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="16" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="16" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="16" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="8" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="8" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="16" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="16" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="16" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="16" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="16" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -16252,38 +16258,39 @@
     <hyperlink r:id="rId38" ref="G7"/>
     <hyperlink r:id="rId39" ref="B8"/>
     <hyperlink r:id="rId40" ref="C8"/>
-    <hyperlink r:id="rId41" ref="G8"/>
-    <hyperlink r:id="rId42" ref="B9"/>
-    <hyperlink r:id="rId43" ref="C9"/>
-    <hyperlink r:id="rId44" ref="G9"/>
-    <hyperlink r:id="rId45" ref="B10"/>
-    <hyperlink r:id="rId46" ref="C10"/>
-    <hyperlink r:id="rId47" ref="G10"/>
-    <hyperlink r:id="rId48" ref="C11"/>
-    <hyperlink r:id="rId49" ref="G11"/>
-    <hyperlink r:id="rId50" ref="C12"/>
-    <hyperlink r:id="rId51" ref="G12"/>
-    <hyperlink r:id="rId52" ref="C13"/>
-    <hyperlink r:id="rId53" ref="G13"/>
-    <hyperlink r:id="rId54" ref="C14"/>
-    <hyperlink r:id="rId55" ref="G14"/>
-    <hyperlink r:id="rId56" ref="C15"/>
-    <hyperlink r:id="rId57" ref="G15"/>
-    <hyperlink r:id="rId58" ref="C16"/>
-    <hyperlink r:id="rId59" ref="G16"/>
-    <hyperlink r:id="rId60" ref="C17"/>
-    <hyperlink r:id="rId61" ref="G17"/>
-    <hyperlink r:id="rId62" ref="C18"/>
-    <hyperlink r:id="rId63" ref="G18"/>
-    <hyperlink r:id="rId64" ref="C19"/>
-    <hyperlink r:id="rId65" ref="G19"/>
-    <hyperlink r:id="rId66" ref="C20"/>
-    <hyperlink r:id="rId67" ref="G20"/>
-    <hyperlink r:id="rId68" ref="C21"/>
-    <hyperlink r:id="rId69" ref="C22"/>
-    <hyperlink r:id="rId70" ref="C23"/>
+    <hyperlink r:id="rId41" ref="D8"/>
+    <hyperlink r:id="rId42" ref="G8"/>
+    <hyperlink r:id="rId43" ref="B9"/>
+    <hyperlink r:id="rId44" ref="C9"/>
+    <hyperlink r:id="rId45" ref="G9"/>
+    <hyperlink r:id="rId46" ref="B10"/>
+    <hyperlink r:id="rId47" ref="C10"/>
+    <hyperlink r:id="rId48" ref="G10"/>
+    <hyperlink r:id="rId49" ref="C11"/>
+    <hyperlink r:id="rId50" ref="G11"/>
+    <hyperlink r:id="rId51" ref="C12"/>
+    <hyperlink r:id="rId52" ref="G12"/>
+    <hyperlink r:id="rId53" ref="C13"/>
+    <hyperlink r:id="rId54" ref="G13"/>
+    <hyperlink r:id="rId55" ref="C14"/>
+    <hyperlink r:id="rId56" ref="G14"/>
+    <hyperlink r:id="rId57" ref="C15"/>
+    <hyperlink r:id="rId58" ref="G15"/>
+    <hyperlink r:id="rId59" ref="C16"/>
+    <hyperlink r:id="rId60" ref="G16"/>
+    <hyperlink r:id="rId61" ref="C17"/>
+    <hyperlink r:id="rId62" ref="G17"/>
+    <hyperlink r:id="rId63" ref="C18"/>
+    <hyperlink r:id="rId64" ref="G18"/>
+    <hyperlink r:id="rId65" ref="C19"/>
+    <hyperlink r:id="rId66" ref="G19"/>
+    <hyperlink r:id="rId67" ref="C20"/>
+    <hyperlink r:id="rId68" ref="G20"/>
+    <hyperlink r:id="rId69" ref="C21"/>
+    <hyperlink r:id="rId70" ref="C22"/>
+    <hyperlink r:id="rId71" ref="C23"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId72"/>
 </worksheet>
 </file>
 
@@ -16305,7 +16312,7 @@
         <v>774</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>773</v>
@@ -16322,13 +16329,13 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>759</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>763</v>
@@ -16337,15 +16344,15 @@
         <v>758</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="8" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>760</v>
@@ -16356,7 +16363,7 @@
     </row>
     <row r="4">
       <c r="E4" s="16" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>769</v>
@@ -16364,7 +16371,7 @@
     </row>
     <row r="5">
       <c r="E5" s="8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="6">
@@ -16374,12 +16381,12 @@
     </row>
     <row r="7">
       <c r="E7" s="8" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" s="8" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -16423,7 +16430,7 @@
         <v>774</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>773</v>
@@ -16440,122 +16447,122 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>761</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="20"/>
       <c r="E5" s="8" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" s="8" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="7">
       <c r="E7" s="8" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" s="8" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
     </row>
     <row r="9">
       <c r="E9" s="8" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="10">
       <c r="E10" s="8" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="11">
       <c r="E11" s="16" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="12">
       <c r="E12" s="8" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="13">
       <c r="E13" s="8" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="14">
       <c r="E14" s="8" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="15">
       <c r="E15" s="8" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="16">
       <c r="E16" s="16" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="17">
       <c r="E17" s="8" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="37">
@@ -16626,42 +16633,42 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
   </sheetData>
@@ -16705,7 +16712,7 @@
         <v>773</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>774</v>
@@ -16740,25 +16747,25 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -16784,20 +16791,20 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="21" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -16824,17 +16831,17 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="21" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -16861,11 +16868,11 @@
     </row>
     <row r="5">
       <c r="C5" s="21" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="21" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>788</v>
@@ -16895,7 +16902,7 @@
     </row>
     <row r="6">
       <c r="C6" s="21" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -16927,14 +16934,14 @@
     </row>
     <row r="7">
       <c r="C7" s="21" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="21" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -46752,74 +46759,74 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="16" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="16" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="16" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="8" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="8" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="16" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="16" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="16" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
     </row>
   </sheetData>
@@ -46873,21 +46880,21 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>762</v>
@@ -46895,15 +46902,15 @@
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="8" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refine the smell examples
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboards.xlsx
+++ b/meta/Foundation Model Leaderboards.xlsx
@@ -2402,7 +2402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="908">
   <si>
     <t>Name</t>
   </si>
@@ -4606,16 +4606,16 @@
     <t>Benchmark Raw Dataset</t>
   </si>
   <si>
-    <t>Evaluation Record</t>
-  </si>
-  <si>
-    <t>Model</t>
+    <t>Evaluation Record/Result</t>
+  </si>
+  <si>
+    <t>Model (Information)</t>
   </si>
   <si>
     <t>Ranking Dataframe</t>
   </si>
   <si>
-    <t>Submission Channel</t>
+    <t>Submission Channel/Guideline</t>
   </si>
   <si>
     <t>https://github.com/CLUEbenchmark/SuperCLUE-Code3/issues/2</t>
@@ -5005,19 +5005,22 @@
     <t>https://huggingface.co/spaces/mlabonne/Yet_Another_LLM_Leaderboard/discussions/11</t>
   </si>
   <si>
+    <t>https://github.com/Re-Align/URIAL/issues/7</t>
+  </si>
+  <si>
+    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/10</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/8</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/CathieDaDa/LLM_leaderboard/discussions/2</t>
   </si>
   <si>
-    <t>https://github.com/LudwigStumpp/llm-leaderboard/issues/10</t>
-  </si>
-  <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/8</t>
+    <t>https://github.com/TabbyML/tabby/issues/1369</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/FinancialSupport/open_ita_llm_leaderboard/discussions/7</t>
-  </si>
-  <si>
-    <t>https://github.com/TabbyML/tabby/issues/1369</t>
   </si>
   <si>
     <t>https://github.com/X-PLUG/Youku-mPLUG/issues/23</t>
@@ -15197,15 +15200,15 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -15233,22 +15236,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="22" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="24" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="5">
@@ -15258,12 +15261,12 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="8">
@@ -15273,7 +15276,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="10">
@@ -16327,7 +16330,7 @@
       <c r="A4" s="21" t="s">
         <v>862</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="9" t="s">
         <v>863</v>
       </c>
       <c r="D4" s="23"/>
@@ -16395,9 +16398,12 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6">
+      <c r="C6" s="21" t="s">
+        <v>868</v>
+      </c>
       <c r="D6" s="23"/>
       <c r="E6" s="21" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>724</v>
@@ -16428,10 +16434,10 @@
     <row r="7">
       <c r="D7" s="23"/>
       <c r="E7" s="21" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -46209,13 +46215,14 @@
     <hyperlink r:id="rId18" ref="C5"/>
     <hyperlink r:id="rId19" ref="E5"/>
     <hyperlink r:id="rId20" ref="F5"/>
-    <hyperlink r:id="rId21" ref="E6"/>
-    <hyperlink r:id="rId22" ref="F6"/>
-    <hyperlink r:id="rId23" ref="E7"/>
-    <hyperlink r:id="rId24" ref="F7"/>
+    <hyperlink r:id="rId21" ref="C6"/>
+    <hyperlink r:id="rId22" ref="E6"/>
+    <hyperlink r:id="rId23" ref="F6"/>
+    <hyperlink r:id="rId24" ref="E7"/>
+    <hyperlink r:id="rId25" ref="F7"/>
   </hyperlinks>
-  <drawing r:id="rId25"/>
-  <legacyDrawing r:id="rId26"/>
+  <drawing r:id="rId26"/>
+  <legacyDrawing r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -46248,29 +46255,29 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="17" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="17" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>715</v>
@@ -46278,51 +46285,51 @@
     </row>
     <row r="5">
       <c r="B5" s="9" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="17" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="17" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="17" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="9" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="17" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
   </sheetData>
@@ -46377,21 +46384,21 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>716</v>
@@ -46399,15 +46406,15 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="9" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more smell examples
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboards.xlsx
+++ b/meta/Foundation Model Leaderboards.xlsx
@@ -2431,7 +2431,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="1009">
   <si>
     <t>Name</t>
   </si>
@@ -4641,6 +4641,9 @@
     <t>https://huggingface.co/spaces/BramVanroy/open_dutch_llm_leaderboard</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/choco9966/open-ko-llm-leaderboard/discussions/2</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/felixz/meta_open_llm_leaderboard/discussions/1</t>
   </si>
   <si>
@@ -5163,16 +5166,115 @@
     <t>https://huggingface.co/spaces/Vchitect/VBench/discussions/1</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/0x1668/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://github.com/THU-KEG/KoLA/issues/17</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/0x9/finetuning_subnet_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/openlifescienceai/open_medical_llm_leaderboard/discussions/17</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/0x9/pretraining-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Aarifkhan/leaderboard-results-to-modelcard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/abidlabs/chatbot-arena-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/abidlabs/mteb-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/AI-Vietnam/prompt-translation-vie-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Alfasign/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard-docker/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard-gradio/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/arshy/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/asir0z/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/automerger/Yet_Another_LLM_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/awacke1/CanAICode-Leaderboard-Customized/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/b1sheng/kg_llm_leaderboard_test/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/bittensor-dataset/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/CDT-BMAI-GP/biomed_probing_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/choco9966/LeaderboardTest/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/Classroom-workshop/assignments-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/CVPR/Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/DeepBrainz/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/demo-crafters/leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/demo-leaderboard-backend/leaderboard/discussions/6</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/demo-leaderboard/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard-v13/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/deprem-ml/intent-leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/dimbyTa/open-llm-leaderboard-viz/discussions/1</t>
   </si>
   <si>
-    <t>https://github.com/THU-KEG/KoLA/issues/17</t>
+    <t>https://huggingface.co/spaces/Docfile/open_llm_leaderboard/discussions/1</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/DontPlanToEnd/UGI-Leaderboard/discussions/4</t>
   </si>
   <si>
-    <t>https://huggingface.co/spaces/openlifescienceai/open_medical_llm_leaderboard/discussions/17</t>
+    <t>https://huggingface.co/spaces/ecai-2034/FSS-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ECCV2022/Leaderboard/discussions/2</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/eduagarcia-temp/portuguese-leaderboard-results-to-modelcard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/EuroPython2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/EuroSciPy2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/freddyaboulton/gradio_leaderboard_demo/discussions/1</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/gaia-benchmark/leaderboard/discussions/14</t>
@@ -5181,12 +5283,57 @@
     <t>https://huggingface.co/spaces/glitchbench/Leaderboard/discussions/3</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/Gradio-Blocks/Leaderboard/discussions/3</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/hjzhou/chatbot-arena-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/homunculus/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/HuggingFaceH4/human_eval_llm_leaderboard/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ICML2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/JarvisKi/Stable_Tool_Bench_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/kbmlcoding/open_llm_leaderboard_free/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/khhuiyh/AutoEval-Video_LeaderBoard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/kunato-lab/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ludwigstumpp/llm-leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/MarketingHackers/chatbot-arena-leaderboard/discussions/1</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/mlfoundations/VisIT-Bench-Leaderboard/discussions/2</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/NAACL2022/Spaces-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nan/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/neelalex/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nlphuji/WHOOPS-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/nouamanetazi/mteb-leaderboard-old/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/opencompass/open_vlm_leaderboard/discussions/7</t>
   </si>
   <si>
@@ -5199,16 +5346,106 @@
     <t>https://huggingface.co/spaces/openlifescienceai/open_medical_llm_leaderboard/discussions/2</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/openskyml/diffusion-models-leaderboard-template/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/osanseviero/llama-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/patrickvonplaten/parti-prompts-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/platzi/platzi-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/PlixAI/pixel-subnet-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard_two/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/pngwn/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/RaoFoundation/pretraining-leaderboard/discussions/1</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/reach-vb/leaderboards/discussions/4</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_enterprise_scenarios_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_hallucination_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_llm_perf_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data_only_open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rodrigomasini/data-only-mteb-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/rusticluftig/9-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/sanchit-gandhi/leaderboards/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/seikwan/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/SIGGRAPH2022/Leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/Skywork/agent-studio-leaderboard/discussions/1</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/smothiki/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/somosnlp/likes_leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/sparse-generative-ai/open-moe-llm-leaderboard/discussions/1</t>
   </si>
   <si>
+    <t>https://huggingface.co/spaces/speech-recognition-community-v2/Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/stabletoolbench/Stable_Tool_Bench_Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/starmorph/open_llm_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard-test/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ThomasSimonini/Deep-Reinforcement-Learning-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/TIGER-Lab/LongICL-Leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/umdclip/grounded_qa_leaderboard/discussions/1</t>
+  </si>
+  <si>
     <t>https://huggingface.co/spaces/valory/olas-prediction-leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/winglian/finetuning_subnet_leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/xtreme-s/leaderboard/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/ybjeong/leaderboard_kr/discussions/1</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/yzeng58/CoBSAT_Leaderboard/discussions/1</t>
   </si>
   <si>
     <t>Uncategorized</t>
@@ -15399,96 +15636,501 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="18" t="s">
-        <v>908</v>
+      <c r="A3" s="9" t="s">
+        <v>909</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>911</v>
+      <c r="A5" s="18" t="s">
+        <v>912</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="18" t="s">
-        <v>893</v>
+      <c r="A6" s="9" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>913</v>
+      <c r="A8" s="18" t="s">
+        <v>915</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>915</v>
+      <c r="A10" s="18" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>916</v>
+      <c r="A11" s="18" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>917</v>
+      <c r="A12" s="18" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>918</v>
+      <c r="A13" s="9" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="18" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
-        <v>921</v>
+      <c r="A16" s="18" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="18" t="s">
-        <v>905</v>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="18" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="18" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="18" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="18" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="18" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="18" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="18" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="18" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="18" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="18" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="18" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="9" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="18" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="18" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="18" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="18" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="18" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="18" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="18" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="18" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="9" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="9" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="18" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="9" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="18" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="18" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="18" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="18" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="18" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="18" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="9" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="18" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="18" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="9" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="18" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="18" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="18" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="18" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="18" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="9" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="9" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="9" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="9" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="18" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="9" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="18" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="18" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="18" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="18" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="18" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="18" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="18" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="18" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="18" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="18" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="18" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="18" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="18" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="18" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="18" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="18" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="18" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="18" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="18" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="18" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="18" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="9" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="18" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="18" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="18" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="18" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="18" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="18" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="9" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="18" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="18" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="18" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="18" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="18" t="s">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -15511,8 +16153,89 @@
     <hyperlink r:id="rId16" ref="A15"/>
     <hyperlink r:id="rId17" ref="A16"/>
     <hyperlink r:id="rId18" ref="A17"/>
+    <hyperlink r:id="rId19" ref="A18"/>
+    <hyperlink r:id="rId20" ref="A19"/>
+    <hyperlink r:id="rId21" ref="A20"/>
+    <hyperlink r:id="rId22" ref="A21"/>
+    <hyperlink r:id="rId23" ref="A22"/>
+    <hyperlink r:id="rId24" ref="A23"/>
+    <hyperlink r:id="rId25" ref="A24"/>
+    <hyperlink r:id="rId26" ref="A25"/>
+    <hyperlink r:id="rId27" ref="A26"/>
+    <hyperlink r:id="rId28" ref="A27"/>
+    <hyperlink r:id="rId29" ref="A28"/>
+    <hyperlink r:id="rId30" ref="A29"/>
+    <hyperlink r:id="rId31" ref="A30"/>
+    <hyperlink r:id="rId32" ref="A31"/>
+    <hyperlink r:id="rId33" ref="A32"/>
+    <hyperlink r:id="rId34" ref="A33"/>
+    <hyperlink r:id="rId35" ref="A34"/>
+    <hyperlink r:id="rId36" ref="A35"/>
+    <hyperlink r:id="rId37" ref="A36"/>
+    <hyperlink r:id="rId38" ref="A37"/>
+    <hyperlink r:id="rId39" ref="A38"/>
+    <hyperlink r:id="rId40" ref="A39"/>
+    <hyperlink r:id="rId41" ref="A40"/>
+    <hyperlink r:id="rId42" ref="A41"/>
+    <hyperlink r:id="rId43" ref="A42"/>
+    <hyperlink r:id="rId44" ref="A43"/>
+    <hyperlink r:id="rId45" ref="A44"/>
+    <hyperlink r:id="rId46" ref="A45"/>
+    <hyperlink r:id="rId47" ref="A46"/>
+    <hyperlink r:id="rId48" ref="A47"/>
+    <hyperlink r:id="rId49" ref="A48"/>
+    <hyperlink r:id="rId50" ref="A49"/>
+    <hyperlink r:id="rId51" ref="A50"/>
+    <hyperlink r:id="rId52" ref="A51"/>
+    <hyperlink r:id="rId53" ref="A52"/>
+    <hyperlink r:id="rId54" ref="A53"/>
+    <hyperlink r:id="rId55" ref="A54"/>
+    <hyperlink r:id="rId56" ref="A55"/>
+    <hyperlink r:id="rId57" ref="A56"/>
+    <hyperlink r:id="rId58" ref="A57"/>
+    <hyperlink r:id="rId59" ref="A58"/>
+    <hyperlink r:id="rId60" ref="A59"/>
+    <hyperlink r:id="rId61" ref="A60"/>
+    <hyperlink r:id="rId62" ref="A61"/>
+    <hyperlink r:id="rId63" ref="A62"/>
+    <hyperlink r:id="rId64" ref="A63"/>
+    <hyperlink r:id="rId65" ref="A64"/>
+    <hyperlink r:id="rId66" ref="A65"/>
+    <hyperlink r:id="rId67" ref="A66"/>
+    <hyperlink r:id="rId68" ref="A67"/>
+    <hyperlink r:id="rId69" ref="A68"/>
+    <hyperlink r:id="rId70" ref="A69"/>
+    <hyperlink r:id="rId71" ref="A70"/>
+    <hyperlink r:id="rId72" ref="A71"/>
+    <hyperlink r:id="rId73" ref="A72"/>
+    <hyperlink r:id="rId74" ref="A73"/>
+    <hyperlink r:id="rId75" ref="A74"/>
+    <hyperlink r:id="rId76" ref="A75"/>
+    <hyperlink r:id="rId77" ref="A76"/>
+    <hyperlink r:id="rId78" ref="A77"/>
+    <hyperlink r:id="rId79" ref="A78"/>
+    <hyperlink r:id="rId80" ref="A79"/>
+    <hyperlink r:id="rId81" ref="A80"/>
+    <hyperlink r:id="rId82" ref="A81"/>
+    <hyperlink r:id="rId83" ref="A82"/>
+    <hyperlink r:id="rId84" ref="A83"/>
+    <hyperlink r:id="rId85" ref="A84"/>
+    <hyperlink r:id="rId86" ref="A85"/>
+    <hyperlink r:id="rId87" ref="A86"/>
+    <hyperlink r:id="rId88" ref="A87"/>
+    <hyperlink r:id="rId89" ref="A88"/>
+    <hyperlink r:id="rId90" ref="A89"/>
+    <hyperlink r:id="rId91" ref="A90"/>
+    <hyperlink r:id="rId92" ref="A91"/>
+    <hyperlink r:id="rId93" ref="A92"/>
+    <hyperlink r:id="rId94" ref="A93"/>
+    <hyperlink r:id="rId95" ref="A94"/>
+    <hyperlink r:id="rId96" ref="A95"/>
+    <hyperlink r:id="rId97" ref="A96"/>
+    <hyperlink r:id="rId98" ref="A97"/>
+    <hyperlink r:id="rId99" ref="A98"/>
   </hyperlinks>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId100"/>
 </worksheet>
 </file>
 
@@ -15531,22 +16254,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="s">
-        <v>922</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>923</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="25" t="s">
-        <v>924</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>925</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5">
@@ -15556,12 +16279,12 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>926</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>927</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="8">
@@ -15571,7 +16294,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>928</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="10">
@@ -15581,12 +16304,12 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>929</v>
+        <v>1008</v>
       </c>
     </row>
   </sheetData>
@@ -15668,7 +16391,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="18" t="s">
         <v>732</v>
       </c>
     </row>
@@ -15678,12 +16401,12 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="9" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="18" t="s">
         <v>735</v>
       </c>
     </row>
@@ -15693,8 +16416,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="9" t="s">
         <v>737</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18" t="s">
+        <v>738</v>
       </c>
     </row>
   </sheetData>
@@ -15715,8 +16443,9 @@
     <hyperlink r:id="rId14" ref="A14"/>
     <hyperlink r:id="rId15" ref="A15"/>
     <hyperlink r:id="rId16" ref="A16"/>
+    <hyperlink r:id="rId17" ref="A17"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -15738,290 +16467,290 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="18" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="9" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="9" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="9" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="9" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="13">
       <c r="C13" s="9" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="18" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="18" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="18" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="17">
       <c r="C17" s="18" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="20">
       <c r="C20" s="18" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="18" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="18" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="18" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" s="18" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -16119,27 +16848,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>740</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>728</v>
@@ -16148,12 +16877,12 @@
         <v>722</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="9" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>724</v>
@@ -16164,18 +16893,18 @@
     </row>
     <row r="4">
       <c r="B4" s="18" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="5">
       <c r="D5" s="9" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="6">
@@ -16185,12 +16914,12 @@
     </row>
     <row r="7">
       <c r="D7" s="9" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" s="9" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
   </sheetData>
@@ -16230,123 +16959,123 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>740</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="D5" s="9" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="6">
       <c r="D6" s="9" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="7">
       <c r="D7" s="9" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" s="9" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="9">
       <c r="D9" s="9" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="10">
       <c r="D10" s="9" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" s="18" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" s="9" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="13">
       <c r="D13" s="9" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="14">
       <c r="D14" s="9" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="15">
       <c r="D15" s="9" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="16">
@@ -16405,53 +17134,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -16486,25 +17215,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -16530,25 +17259,25 @@
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -16574,20 +17303,20 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="22" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -16614,17 +17343,17 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="22" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -16651,14 +17380,14 @@
     </row>
     <row r="5">
       <c r="C5" s="22" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="22" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -16685,14 +17414,14 @@
     </row>
     <row r="6">
       <c r="C6" s="22" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="22" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -16720,10 +17449,10 @@
     <row r="7">
       <c r="D7" s="24"/>
       <c r="E7" s="22" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -46527,43 +47256,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="18" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="18" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>726</v>
@@ -46571,51 +47300,51 @@
     </row>
     <row r="5">
       <c r="B5" s="9" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="9" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="18" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="18" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="18" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="18" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="9" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
     <row r="12">
       <c r="C12" s="18" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -46659,32 +47388,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>727</v>
@@ -46692,15 +47421,15 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="9" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refine figure for teaser
</commit_message>
<xml_diff>
--- a/meta/Foundation Model Leaderboards.xlsx
+++ b/meta/Foundation Model Leaderboards.xlsx
@@ -6093,13 +6093,13 @@
     <t>https://github.com/HowieHwong/TrustLLM/pull/13</t>
   </si>
   <si>
-    <t>https://github.com/microsoft/promptbench/issues/52</t>
-  </si>
-  <si>
     <t>https://github.com/microsoft/promptbench/issues/59</t>
   </si>
   <si>
     <t>https://github.com/open-compass/MathBench/issues/5</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/spaces/archit11/Hindi_LLM_arena/discussions/1</t>
   </si>
   <si>
     <t>https://huggingface.co/spaces/CathieDaDa/LLM_leaderboard/discussions/2</t>
@@ -17106,43 +17106,43 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="24" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="28" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="28" t="s">
-        <v>750</v>
-      </c>
-    </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>1057</v>
+      <c r="A15" s="24" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="24" t="s">
-        <v>756</v>
+      <c r="A17" s="3" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>760</v>
+      <c r="A18" s="24" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
-        <v>761</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="20">

</xml_diff>